<commit_message>
add mode selection(DBG or UMS)
</commit_message>
<xml_diff>
--- a/doc/BOM.xlsx
+++ b/doc/BOM.xlsx
@@ -225,9 +225,6 @@
     <t>R-0603(1608),100K</t>
   </si>
   <si>
-    <t>R1 R7 R16-17 R27 R35 R37-43 R48 R53-54 R58</t>
-  </si>
-  <si>
     <t>R-0603(1608),10K</t>
   </si>
   <si>
@@ -431,6 +428,10 @@
   </si>
   <si>
     <t>3x5 size</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>R1 R7 R16-17 R27 R35 R37-43 R48 R53-54 R58 R60-61</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1568,7 +1569,7 @@
   <dimension ref="B1:F57"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="F55" sqref="F55"/>
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1595,7 +1596,7 @@
         <v>3</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.3">
@@ -1642,7 +1643,7 @@
         <v>9</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.3">
@@ -1659,7 +1660,7 @@
         <v>11</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.3">
@@ -1676,7 +1677,7 @@
         <v>13</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.3">
@@ -1693,7 +1694,7 @@
         <v>15</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.3">
@@ -1845,7 +1846,7 @@
         <v>35</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.3">
@@ -1862,7 +1863,7 @@
         <v>37</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.3">
@@ -1879,7 +1880,7 @@
         <v>39</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.3">
@@ -1941,7 +1942,7 @@
         <v>47</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.3">
@@ -2003,7 +2004,7 @@
         <v>55</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.3">
@@ -2035,7 +2036,7 @@
         <v>59</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.3">
@@ -2106,10 +2107,10 @@
         <v>17</v>
       </c>
       <c r="D35" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="E35" s="2" t="s">
         <v>68</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>69</v>
       </c>
       <c r="F35" s="3"/>
     </row>
@@ -2121,10 +2122,10 @@
         <v>1</v>
       </c>
       <c r="D36" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E36" s="2" t="s">
         <v>70</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>71</v>
       </c>
       <c r="F36" s="3"/>
     </row>
@@ -2136,10 +2137,10 @@
         <v>6</v>
       </c>
       <c r="D37" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E37" s="2" t="s">
         <v>72</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>73</v>
       </c>
       <c r="F37" s="3"/>
     </row>
@@ -2151,10 +2152,10 @@
         <v>1</v>
       </c>
       <c r="D38" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E38" s="2" t="s">
         <v>74</v>
-      </c>
-      <c r="E38" s="2" t="s">
-        <v>75</v>
       </c>
       <c r="F38" s="3"/>
     </row>
@@ -2166,10 +2167,10 @@
         <v>1</v>
       </c>
       <c r="D39" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E39" s="2" t="s">
         <v>76</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>77</v>
       </c>
       <c r="F39" s="3"/>
     </row>
@@ -2181,10 +2182,10 @@
         <v>1</v>
       </c>
       <c r="D40" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E40" s="2" t="s">
         <v>78</v>
-      </c>
-      <c r="E40" s="2" t="s">
-        <v>79</v>
       </c>
       <c r="F40" s="3"/>
     </row>
@@ -2196,13 +2197,13 @@
         <v>2</v>
       </c>
       <c r="D41" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E41" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="E41" s="2" t="s">
-        <v>81</v>
-      </c>
       <c r="F41" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="42" spans="2:6" x14ac:dyDescent="0.3">
@@ -2213,10 +2214,10 @@
         <v>1</v>
       </c>
       <c r="D42" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E42" s="2" t="s">
         <v>82</v>
-      </c>
-      <c r="E42" s="2" t="s">
-        <v>83</v>
       </c>
       <c r="F42" s="3"/>
     </row>
@@ -2228,10 +2229,10 @@
         <v>1</v>
       </c>
       <c r="D43" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E43" s="2" t="s">
         <v>84</v>
-      </c>
-      <c r="E43" s="2" t="s">
-        <v>85</v>
       </c>
       <c r="F43" s="3"/>
     </row>
@@ -2243,10 +2244,10 @@
         <v>1</v>
       </c>
       <c r="D44" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E44" s="2" t="s">
         <v>86</v>
-      </c>
-      <c r="E44" s="2" t="s">
-        <v>87</v>
       </c>
       <c r="F44" s="3"/>
     </row>
@@ -2258,10 +2259,10 @@
         <v>1</v>
       </c>
       <c r="D45" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E45" s="2" t="s">
         <v>88</v>
-      </c>
-      <c r="E45" s="2" t="s">
-        <v>89</v>
       </c>
       <c r="F45" s="3"/>
     </row>
@@ -2273,10 +2274,10 @@
         <v>1</v>
       </c>
       <c r="D46" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="E46" s="2" t="s">
         <v>90</v>
-      </c>
-      <c r="E46" s="2" t="s">
-        <v>91</v>
       </c>
       <c r="F46" s="3"/>
     </row>
@@ -2288,10 +2289,10 @@
         <v>2</v>
       </c>
       <c r="D47" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E47" s="2" t="s">
         <v>92</v>
-      </c>
-      <c r="E47" s="2" t="s">
-        <v>93</v>
       </c>
       <c r="F47" s="3"/>
     </row>
@@ -2303,10 +2304,10 @@
         <v>2</v>
       </c>
       <c r="D48" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E48" s="2" t="s">
         <v>94</v>
-      </c>
-      <c r="E48" s="2" t="s">
-        <v>95</v>
       </c>
       <c r="F48" s="3"/>
     </row>
@@ -2318,10 +2319,10 @@
         <v>1</v>
       </c>
       <c r="D49" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="E49" s="2" t="s">
         <v>96</v>
-      </c>
-      <c r="E49" s="2" t="s">
-        <v>97</v>
       </c>
       <c r="F49" s="3"/>
     </row>
@@ -2333,13 +2334,13 @@
         <v>1</v>
       </c>
       <c r="D50" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E50" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="E50" s="2" t="s">
-        <v>99</v>
-      </c>
       <c r="F50" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="51" spans="2:6" x14ac:dyDescent="0.3">
@@ -2350,10 +2351,10 @@
         <v>1</v>
       </c>
       <c r="D51" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E51" s="2" t="s">
         <v>100</v>
-      </c>
-      <c r="E51" s="2" t="s">
-        <v>101</v>
       </c>
       <c r="F51" s="3"/>
     </row>
@@ -2365,13 +2366,13 @@
         <v>2</v>
       </c>
       <c r="D52" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="E52" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="E52" s="2" t="s">
-        <v>103</v>
-      </c>
       <c r="F52" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="53" spans="2:6" x14ac:dyDescent="0.3">
@@ -2382,13 +2383,13 @@
         <v>1</v>
       </c>
       <c r="D53" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="E53" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="E53" s="2" t="s">
-        <v>105</v>
-      </c>
       <c r="F53" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="54" spans="2:6" x14ac:dyDescent="0.3">
@@ -2399,10 +2400,10 @@
         <v>1</v>
       </c>
       <c r="D54" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E54" s="2" t="s">
         <v>106</v>
-      </c>
-      <c r="E54" s="2" t="s">
-        <v>107</v>
       </c>
       <c r="F54" s="3"/>
     </row>
@@ -2414,13 +2415,13 @@
         <v>3</v>
       </c>
       <c r="D55" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E55" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="E55" s="2" t="s">
-        <v>109</v>
-      </c>
       <c r="F55" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="56" spans="2:6" x14ac:dyDescent="0.3">
@@ -2431,13 +2432,13 @@
         <v>1</v>
       </c>
       <c r="D56" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="E56" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="E56" s="2" t="s">
-        <v>111</v>
-      </c>
       <c r="F56" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="57" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -2448,13 +2449,13 @@
         <v>1</v>
       </c>
       <c r="D57" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="E57" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="E57" s="5" t="s">
-        <v>113</v>
-      </c>
       <c r="F57" s="6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>

</xml_diff>